<commit_message>
Ajout description des blocs
</commit_message>
<xml_diff>
--- a/data_description.xlsx
+++ b/data_description.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erwan/Documents/Cours/Master/M2/db_spe/bitcoin-blockchain-neo4j/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6035F32-200D-4A4E-A6D7-10A36C01D3AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E56A6D0-F12A-544E-98D8-011617F8CF26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="20900" xr2:uid="{FE4CE8A4-3171-9042-99C3-3AE1ADC9B379}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="95">
   <si>
     <t>Description de la transaction</t>
   </si>
@@ -287,12 +287,84 @@
 - Blocs : https://github.com/blockchain-etl/bitcoin-etl-airflow/blob/master/dags/resources/stages/enrich/schemas/blocks.json</t>
     </r>
   </si>
+  <si>
+    <t>REQUIRED</t>
+  </si>
+  <si>
+    <t>Description bloc</t>
+  </si>
+  <si>
+    <t>stripped_size</t>
+  </si>
+  <si>
+    <t>weight</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>markle_root</t>
+  </si>
+  <si>
+    <t>timestamp_month</t>
+  </si>
+  <si>
+    <t>nonce</t>
+  </si>
+  <si>
+    <t>bits</t>
+  </si>
+  <si>
+    <t>coinbase_param</t>
+  </si>
+  <si>
+    <t>transaction_count</t>
+  </si>
+  <si>
+    <t>Hash du bloc</t>
+  </si>
+  <si>
+    <t>Taille des données du blocs en bytes (octets)</t>
+  </si>
+  <si>
+    <t>Taille des données du blocs en bytes (octets) en excluant les données témoins ('witness data')</t>
+  </si>
+  <si>
+    <t>Poids : 3*stripped_size + size (https://github.com/bitcoin/bips/blob/master/bip-0141.mediawiki)</t>
+  </si>
+  <si>
+    <t>Numéro du bloc</t>
+  </si>
+  <si>
+    <t>Version du protocol (spécifiée dans le header du bloc)</t>
+  </si>
+  <si>
+    <t>Nœud racine dans l'arbre de Merkle ('Merkle tree') où les feuilles sont des hash de transactions</t>
+  </si>
+  <si>
+    <t>Timestamp de création du bloc (spacifié dans le header du bloc)</t>
+  </si>
+  <si>
+    <t>Mois du timestamp de création du bloc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Difficulty solution specified in block header' </t>
+  </si>
+  <si>
+    <t>Seuil de difficulté ('Difficulty threshold') présent dans le header du bloc</t>
+  </si>
+  <si>
+    <t>('Data specified in the coinbase transaction of this block')</t>
+  </si>
+  <si>
+    <t>Nombre de transactions contenues dans le bloc</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -311,6 +383,13 @@
       <color theme="1"/>
       <name val="Calibri (Corps)"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -320,7 +399,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -463,21 +542,54 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -487,9 +599,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -804,574 +935,776 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC049247-0F1D-3F42-AED2-0B4B8A30F3BE}">
-  <dimension ref="A1:N39"/>
+  <dimension ref="A1:T40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.83203125" customWidth="1"/>
-    <col min="2" max="2" width="16.5" customWidth="1"/>
-    <col min="3" max="3" width="82" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="81.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
+    <col min="17" max="17" width="21.6640625" customWidth="1"/>
+    <col min="18" max="18" width="16.6640625" customWidth="1"/>
+    <col min="19" max="19" width="81.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:20" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="4"/>
-      <c r="E1" s="11" t="s">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="13"/>
+      <c r="F1" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+    </row>
+    <row r="2" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
+      <c r="D2" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
+      <c r="Q2" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="R2" s="12"/>
+      <c r="S2" s="12"/>
+      <c r="T2" s="20"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+      <c r="D3" s="4"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="Q3" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="R3" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="S3" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="T3" s="16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="11"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
+      <c r="D4" s="4"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="Q4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="T4" s="4"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="11"/>
-    </row>
-    <row r="6" spans="1:14" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
+      <c r="D5" s="4"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
+      <c r="Q5" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="T5" s="4"/>
+    </row>
+    <row r="6" spans="1:20" ht="34" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="11"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
+      <c r="D6" s="5"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+      <c r="Q6" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="T6" s="4"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="11"/>
-      <c r="N7" s="11"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
+      <c r="D7" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="Q7" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="T7" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
-      <c r="M8" s="11"/>
-      <c r="N8" s="11"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
+      <c r="D8" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="Q8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="T8" s="4"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="11"/>
-      <c r="M9" s="11"/>
-      <c r="N9" s="11"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
+      <c r="D9" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+      <c r="Q9" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="T9" s="4"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="11"/>
-      <c r="M10" s="11"/>
-      <c r="N10" s="11"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
+      <c r="D10" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="Q10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="T10" s="19" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="11"/>
-      <c r="M11" s="11"/>
-      <c r="N11" s="11"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
+      <c r="D11" s="4"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="Q11" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="T11" s="19" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="11"/>
-      <c r="M12" s="11"/>
-      <c r="N12" s="11"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
+      <c r="D12" s="4"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="Q12" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="S12" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="T12" s="4"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="11"/>
-      <c r="L13" s="11"/>
-      <c r="M13" s="11"/>
-      <c r="N13" s="11"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
+      <c r="D13" s="4"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
+      <c r="Q13" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="R13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="S13" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="T13" s="4"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="11"/>
-      <c r="M14" s="11"/>
-      <c r="N14" s="11"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
+      <c r="D14" s="4"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10"/>
+      <c r="Q14" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="R14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="S14" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="T14" s="4"/>
+    </row>
+    <row r="15" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="11"/>
-      <c r="M15" s="11"/>
-      <c r="N15" s="11"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
+      <c r="D15" s="4"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
+      <c r="Q15" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="R15" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="S15" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="T15" s="8"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="7" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
+      <c r="D18" s="8"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+    </row>
+    <row r="20" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="4"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="5" t="s">
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="13"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B22" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C22" s="15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
+      <c r="D22" s="16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C23" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="5" t="s">
+      <c r="D23" s="4"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C24" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="5" t="s">
+      <c r="D24" s="4"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="5" t="s">
-        <v>52</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D25" s="4"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A26" s="5" t="s">
+      <c r="D26" s="4"/>
+    </row>
+    <row r="27" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A27" s="5" t="s">
-        <v>55</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C27" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D27" s="5"/>
+    </row>
+    <row r="28" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="5" t="s">
+      <c r="D28" s="5"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B29" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C29" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="5" t="s">
+      <c r="D29" s="4"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C30" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="8" t="s">
+      <c r="D30" s="4"/>
+    </row>
+    <row r="31" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="B30" s="9" t="s">
+      <c r="B31" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="C31" s="7" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
+      <c r="D31" s="8"/>
+    </row>
+    <row r="32" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="B32" s="3"/>
-      <c r="C32" s="4"/>
-    </row>
-    <row r="33" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A33" s="5" t="s">
+      <c r="B33" s="12"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="13"/>
+    </row>
+    <row r="34" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A34" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B34" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="C34" s="17" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="5" t="s">
+      <c r="D34" s="16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="5" t="s">
-        <v>52</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="C35" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D35" s="4"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="5" t="s">
+      <c r="D36" s="4"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B37" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="C37" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="5" t="s">
+      <c r="D37" s="4"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B38" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="C38" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="5" t="s">
+      <c r="D38" s="4"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B39" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C39" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="8" t="s">
+      <c r="D39" s="4"/>
+    </row>
+    <row r="40" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="B39" s="9" t="s">
+      <c r="B40" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C39" s="10" t="s">
+      <c r="C40" s="7" t="s">
         <v>65</v>
       </c>
+      <c r="D40" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="E1:N15"/>
+  <mergeCells count="5">
+    <mergeCell ref="Q2:S2"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="F1:O15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Ajout précision dans la description
</commit_message>
<xml_diff>
--- a/data_description.xlsx
+++ b/data_description.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erwan/Documents/Cours/Master/M2/db_spe/bitcoin-blockchain-neo4j/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E56A6D0-F12A-544E-98D8-011617F8CF26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AAA741B-40A2-8F43-9C1B-D44F80C53819}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="20900" xr2:uid="{FE4CE8A4-3171-9042-99C3-3AE1ADC9B379}"/>
   </bookViews>
@@ -253,6 +253,78 @@
 à cet output précis</t>
   </si>
   <si>
+    <t>REQUIRED</t>
+  </si>
+  <si>
+    <t>Description bloc</t>
+  </si>
+  <si>
+    <t>stripped_size</t>
+  </si>
+  <si>
+    <t>weight</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>markle_root</t>
+  </si>
+  <si>
+    <t>timestamp_month</t>
+  </si>
+  <si>
+    <t>nonce</t>
+  </si>
+  <si>
+    <t>bits</t>
+  </si>
+  <si>
+    <t>coinbase_param</t>
+  </si>
+  <si>
+    <t>transaction_count</t>
+  </si>
+  <si>
+    <t>Hash du bloc</t>
+  </si>
+  <si>
+    <t>Taille des données du blocs en bytes (octets)</t>
+  </si>
+  <si>
+    <t>Taille des données du blocs en bytes (octets) en excluant les données témoins ('witness data')</t>
+  </si>
+  <si>
+    <t>Poids : 3*stripped_size + size (https://github.com/bitcoin/bips/blob/master/bip-0141.mediawiki)</t>
+  </si>
+  <si>
+    <t>Numéro du bloc</t>
+  </si>
+  <si>
+    <t>Version du protocol (spécifiée dans le header du bloc)</t>
+  </si>
+  <si>
+    <t>Nœud racine dans l'arbre de Merkle ('Merkle tree') où les feuilles sont des hash de transactions</t>
+  </si>
+  <si>
+    <t>Timestamp de création du bloc (spacifié dans le header du bloc)</t>
+  </si>
+  <si>
+    <t>Mois du timestamp de création du bloc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Difficulty solution specified in block header' </t>
+  </si>
+  <si>
+    <t>Seuil de difficulté ('Difficulty threshold') présent dans le header du bloc</t>
+  </si>
+  <si>
+    <t>('Data specified in the coinbase transaction of this block')</t>
+  </si>
+  <si>
+    <t>Nombre de transactions contenues dans le bloc</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">Notes:
 </t>
@@ -265,6 +337,7 @@
       </rPr>
       <t xml:space="preserve">- [] est quand on peut répéter les arguments (ie. c'est un genre de tableau ou d'objet json qui peut contenir plusieurs objets)
 - s'il y a des parenthèses avec un bout de phrase en anglais c'est qu'il y avait un doute lors de la traduction
+- la description de inputs/outputs est la descrpition des Records contenus dans les transactions 
 </t>
     </r>
     <r>
@@ -286,78 +359,6 @@
       <t>- Transactions : https://github.com/blockchain-etl/bitcoin-etl-airflow/blob/master/dags/resources/stages/enrich/schemas/transactions.json
 - Blocs : https://github.com/blockchain-etl/bitcoin-etl-airflow/blob/master/dags/resources/stages/enrich/schemas/blocks.json</t>
     </r>
-  </si>
-  <si>
-    <t>REQUIRED</t>
-  </si>
-  <si>
-    <t>Description bloc</t>
-  </si>
-  <si>
-    <t>stripped_size</t>
-  </si>
-  <si>
-    <t>weight</t>
-  </si>
-  <si>
-    <t>number</t>
-  </si>
-  <si>
-    <t>markle_root</t>
-  </si>
-  <si>
-    <t>timestamp_month</t>
-  </si>
-  <si>
-    <t>nonce</t>
-  </si>
-  <si>
-    <t>bits</t>
-  </si>
-  <si>
-    <t>coinbase_param</t>
-  </si>
-  <si>
-    <t>transaction_count</t>
-  </si>
-  <si>
-    <t>Hash du bloc</t>
-  </si>
-  <si>
-    <t>Taille des données du blocs en bytes (octets)</t>
-  </si>
-  <si>
-    <t>Taille des données du blocs en bytes (octets) en excluant les données témoins ('witness data')</t>
-  </si>
-  <si>
-    <t>Poids : 3*stripped_size + size (https://github.com/bitcoin/bips/blob/master/bip-0141.mediawiki)</t>
-  </si>
-  <si>
-    <t>Numéro du bloc</t>
-  </si>
-  <si>
-    <t>Version du protocol (spécifiée dans le header du bloc)</t>
-  </si>
-  <si>
-    <t>Nœud racine dans l'arbre de Merkle ('Merkle tree') où les feuilles sont des hash de transactions</t>
-  </si>
-  <si>
-    <t>Timestamp de création du bloc (spacifié dans le header du bloc)</t>
-  </si>
-  <si>
-    <t>Mois du timestamp de création du bloc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Difficulty solution specified in block header' </t>
-  </si>
-  <si>
-    <t>Seuil de difficulté ('Difficulty threshold') présent dans le header du bloc</t>
-  </si>
-  <si>
-    <t>('Data specified in the coinbase transaction of this block')</t>
-  </si>
-  <si>
-    <t>Nombre de transactions contenues dans le bloc</t>
   </si>
 </sst>
 </file>
@@ -937,8 +938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC049247-0F1D-3F42-AED2-0B4B8A30F3BE}">
   <dimension ref="A1:T40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="S17" sqref="S17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -960,7 +961,7 @@
       <c r="C1" s="12"/>
       <c r="D1" s="13"/>
       <c r="F1" s="10" t="s">
-        <v>70</v>
+        <v>94</v>
       </c>
       <c r="G1" s="10"/>
       <c r="H1" s="10"/>
@@ -983,7 +984,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
@@ -996,7 +997,7 @@
       <c r="N2" s="10"/>
       <c r="O2" s="10"/>
       <c r="Q2" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="R2" s="12"/>
       <c r="S2" s="12"/>
@@ -1030,10 +1031,10 @@
         <v>45</v>
       </c>
       <c r="S3" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="T3" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
@@ -1064,7 +1065,7 @@
         <v>5</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="T4" s="4"/>
     </row>
@@ -1090,11 +1091,11 @@
       <c r="N5" s="10"/>
       <c r="O5" s="10"/>
       <c r="Q5" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="R5" s="1"/>
       <c r="S5" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="T5" s="4"/>
     </row>
@@ -1120,11 +1121,11 @@
       <c r="N6" s="10"/>
       <c r="O6" s="10"/>
       <c r="Q6" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="R6" s="1"/>
       <c r="S6" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="T6" s="4"/>
     </row>
@@ -1139,7 +1140,7 @@
         <v>13</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
@@ -1152,16 +1153,16 @@
       <c r="N7" s="10"/>
       <c r="O7" s="10"/>
       <c r="Q7" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="R7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="T7" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
@@ -1175,7 +1176,7 @@
         <v>15</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
@@ -1194,7 +1195,7 @@
         <v>5</v>
       </c>
       <c r="S8" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="T8" s="4"/>
     </row>
@@ -1209,7 +1210,7 @@
         <v>18</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
@@ -1222,13 +1223,13 @@
       <c r="N9" s="10"/>
       <c r="O9" s="10"/>
       <c r="Q9" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="R9" s="1" t="s">
         <v>45</v>
       </c>
       <c r="S9" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="T9" s="4"/>
     </row>
@@ -1243,7 +1244,7 @@
         <v>21</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
@@ -1262,10 +1263,10 @@
         <v>17</v>
       </c>
       <c r="S10" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="T10" s="19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
@@ -1290,16 +1291,16 @@
       <c r="N11" s="10"/>
       <c r="O11" s="10"/>
       <c r="Q11" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="R11" s="1" t="s">
         <v>20</v>
       </c>
       <c r="S11" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="T11" s="19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
@@ -1324,13 +1325,13 @@
       <c r="N12" s="10"/>
       <c r="O12" s="10"/>
       <c r="Q12" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="R12" s="1" t="s">
         <v>45</v>
       </c>
       <c r="S12" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="T12" s="4"/>
     </row>
@@ -1356,13 +1357,13 @@
       <c r="N13" s="10"/>
       <c r="O13" s="10"/>
       <c r="Q13" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="R13" s="1" t="s">
         <v>45</v>
       </c>
       <c r="S13" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="T13" s="4"/>
     </row>
@@ -1388,13 +1389,13 @@
       <c r="N14" s="10"/>
       <c r="O14" s="10"/>
       <c r="Q14" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="R14" s="1" t="s">
         <v>45</v>
       </c>
       <c r="S14" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="T14" s="4"/>
     </row>
@@ -1420,13 +1421,13 @@
       <c r="N15" s="10"/>
       <c r="O15" s="10"/>
       <c r="Q15" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R15" s="7" t="s">
         <v>5</v>
       </c>
       <c r="S15" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="T15" s="8"/>
     </row>
@@ -1492,7 +1493,7 @@
         <v>43</v>
       </c>
       <c r="D22" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -1623,7 +1624,7 @@
         <v>69</v>
       </c>
       <c r="D34" s="16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>